<commit_message>
Added test cases for bmw.com, completed data sheet and test steps along with updates so that test can be ran through testNG runner. Added more test cases to expedia.com and updated data sheet, testNG runnet and test steps.
</commit_message>
<xml_diff>
--- a/com.expedia/src/test/resources/test_data.xlsx
+++ b/com.expedia/src/test/resources/test_data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yahya\IdeaProjects\SeleniumBootcamp\com.expedia\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06998A4E-5916-488C-A65B-7F0AF531B2DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50638690-420B-4F30-A640-BCCB4FBE0255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{5DC96F64-0600-4540-8EF4-E6AE23C27A48}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="1" xr2:uid="{5DC96F64-0600-4540-8EF4-E6AE23C27A48}"/>
   </bookViews>
   <sheets>
     <sheet name="NewsroomPage" sheetId="1" r:id="rId1"/>
+    <sheet name="Flights" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Assertions</t>
   </si>
@@ -50,16 +51,41 @@
   </si>
   <si>
     <t>Welcome to Out Travel the System</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>South Africa</t>
+  </si>
+  <si>
+    <t>Istanbul</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Rome</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -85,8 +111,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,7 +430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C7C825-8D82-4132-9F2A-6781F4BC04E3}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -440,4 +467,84 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBD6B53B-F225-4991-8640-96EC6D2E7BA0}">
+  <dimension ref="A1:A16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added test cases to expedia.
</commit_message>
<xml_diff>
--- a/com.expedia/src/test/resources/test_data.xlsx
+++ b/com.expedia/src/test/resources/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yahya\IdeaProjects\SeleniumBootcamp\com.expedia\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50638690-420B-4F30-A640-BCCB4FBE0255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D69B7D1F-18F2-45E6-BF31-FF0DA8330307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="1" xr2:uid="{5DC96F64-0600-4540-8EF4-E6AE23C27A48}"/>
+    <workbookView xWindow="4240" yWindow="0" windowWidth="17140" windowHeight="14320" activeTab="1" xr2:uid="{5DC96F64-0600-4540-8EF4-E6AE23C27A48}"/>
   </bookViews>
   <sheets>
     <sheet name="NewsroomPage" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Assertions</t>
   </si>
@@ -69,6 +69,21 @@
   </si>
   <si>
     <t>Rome</t>
+  </si>
+  <si>
+    <t>Milan</t>
+  </si>
+  <si>
+    <t>Madrid</t>
+  </si>
+  <si>
+    <t>Barcelona</t>
+  </si>
+  <si>
+    <t>Sydney</t>
+  </si>
+  <si>
+    <t>Newcastle</t>
   </si>
 </sst>
 </file>
@@ -474,7 +489,7 @@
   <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -518,19 +533,29 @@
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>

</xml_diff>